<commit_message>
Made a change in excel.xlsx
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>год</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>Ответ:  4609, 87</t>
+  </si>
+  <si>
+    <t>f</t>
   </si>
 </sst>
 </file>
@@ -1383,10 +1386,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1872,7 +1875,7 @@
         <v>4609.8692016483546</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>7</v>
       </c>
@@ -1883,7 +1886,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <f>(13*E16-C16*B16)/(13*D16-B16*B16)</f>
         <v>17.796428571428585</v>
@@ -1896,9 +1899,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>